<commit_message>
Final changes for LogixalQA
</commit_message>
<xml_diff>
--- a/Input_files/Actual_testcases/Kaman/LogixalQA/ALL_PAGES/END_TO_END/TC02_Verify_MYACC_RegisteredUser.xlsx
+++ b/Input_files/Actual_testcases/Kaman/LogixalQA/ALL_PAGES/END_TO_END/TC02_Verify_MYACC_RegisteredUser.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\Logixal_QA_Sanity\Input_files\Actual_testcases\Kaman\LogixalQA\ALL_PAGES\END_TO_END\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ROhit\Rohit\Automation\Demo\KAMAN_ReExecuteFailedTcs\KAMAN_ECTEST_IE_SANITY\Input_files\Actual_testcases\Kaman\LogixalQA\ALL_PAGES\END_TO_END\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52A511DA-C0D1-42CF-ADB9-D9449C861747}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E767BD33-CC08-49D2-B781-70959907BCD7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TC02_Verify_MYACC_RegisteredUse" sheetId="1" r:id="rId1"/>
@@ -161,9 +161,6 @@
     <t>$Registered_Password</t>
   </si>
   <si>
-    <t>Logout_RegisteredUser</t>
-  </si>
-  <si>
     <t>Link_acc_RegiseredUser</t>
   </si>
   <si>
@@ -213,6 +210,9 @@
   </si>
   <si>
     <t>Sign Out</t>
+  </si>
+  <si>
+    <t>Purchasing History</t>
   </si>
 </sst>
 </file>
@@ -630,8 +630,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -676,16 +676,16 @@
     <row r="3" spans="1:5" ht="15.75" customHeight="1">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="E3" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1">
@@ -700,16 +700,16 @@
     <row r="5" spans="1:5" ht="15.75" customHeight="1">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1">
@@ -733,13 +733,13 @@
     <row r="8" spans="1:5">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>12</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E8" s="4"/>
     </row>
@@ -749,10 +749,10 @@
         <v>15</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E9" s="4"/>
     </row>
@@ -765,7 +765,7 @@
         <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>13</v>
@@ -780,7 +780,7 @@
         <v>14</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>14</v>
@@ -792,10 +792,10 @@
         <v>15</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E12" s="3"/>
     </row>
@@ -817,7 +817,7 @@
         <v>17</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E14" s="3" t="s">
         <v>17</v>
@@ -829,10 +829,10 @@
         <v>9</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>18</v>
@@ -844,10 +844,10 @@
         <v>15</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E16" s="3"/>
     </row>
@@ -860,7 +860,7 @@
         <v>19</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>19</v>
@@ -875,7 +875,7 @@
         <v>20</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>20</v>
@@ -890,7 +890,7 @@
         <v>21</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>21</v>
@@ -905,7 +905,7 @@
         <v>22</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>22</v>
@@ -920,7 +920,7 @@
         <v>23</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>23</v>
@@ -935,7 +935,7 @@
         <v>24</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>24</v>
@@ -947,10 +947,10 @@
         <v>11</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E23" s="3" t="s">
         <v>25</v>
@@ -962,13 +962,13 @@
         <v>11</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="25" spans="1:5">
@@ -980,7 +980,7 @@
         <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>27</v>
@@ -992,10 +992,10 @@
         <v>11</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>28</v>
@@ -1007,10 +1007,10 @@
         <v>15</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>46</v>
+        <v>28</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E27" s="3"/>
     </row>
@@ -1025,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -1143,8 +1143,8 @@
       <c r="A14" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B14" s="3" t="s">
-        <v>25</v>
+      <c r="B14" s="4" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="1:2">
@@ -1157,10 +1157,10 @@
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -1176,7 +1176,7 @@
         <v>28</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -1237,26 +1237,26 @@
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="B26" s="3" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>